<commit_message>
Added local coordinate transformation and stochastic gradient descent with TDOA optimization
</commit_message>
<xml_diff>
--- a/data/how_to_determine_difference_time_of_arrival.xlsx
+++ b/data/how_to_determine_difference_time_of_arrival.xlsx
@@ -127,7 +127,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -137,10 +137,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -229,10 +225,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -1451,7 +1447,7 @@
     </row>
     <row r="122" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="0"/>
-      <c r="C122" s="3" t="n">
+      <c r="C122" s="0" t="n">
         <v>431.786380193</v>
       </c>
       <c r="D122" s="2" t="n">

</xml_diff>